<commit_message>
se agregar desk pruebas
</commit_message>
<xml_diff>
--- a/requisitos/desk-pruebas.xlsx
+++ b/requisitos/desk-pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\poli-apuestas\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52664090-478E-472F-A53B-8BAA504E1517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D09304-DA46-4049-AA4F-13F78626F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{1EEFC200-8A45-4704-AAE7-4CA5539EFDF4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>Realizar registro de usuarios</t>
   </si>
@@ -207,13 +207,56 @@
   </si>
   <si>
     <t>udfbshjubfdjshbfjdbfjds</t>
+  </si>
+  <si>
+    <t>Campo de valores</t>
+  </si>
+  <si>
+    <t>Evento Guardado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Val 10000</t>
+  </si>
+  <si>
+    <t>Min 50,000 - Max 500,000</t>
+  </si>
+  <si>
+    <t>Min 500,000 - Max 50,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Val 0 - (vacio)</t>
+  </si>
+  <si>
+    <t>Rifa - Apuestas</t>
+  </si>
+  <si>
+    <t>*El valor minimo no sebe ser mayor que el maximo</t>
+  </si>
+  <si>
+    <t>*El valor debe ser obligatorio</t>
+  </si>
+  <si>
+    <t>Venta por persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total ventas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok </t>
+  </si>
+  <si>
+    <t>N° Personas participantes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +276,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,43 +301,61 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC3B59-05E1-442F-9E46-0DCE4C09670D}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,10 +699,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2">
@@ -645,8 +713,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -655,8 +723,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -665,8 +733,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="2">
         <v>2.1</v>
       </c>
@@ -675,8 +743,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="2">
         <v>-34</v>
       </c>
@@ -685,8 +753,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -695,13 +763,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="4">
         <v>100000</v>
       </c>
       <c r="D8" t="s">
@@ -709,9 +777,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D9" t="s">
@@ -719,9 +787,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
@@ -729,9 +797,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D11" t="s">
@@ -739,9 +807,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="9">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4">
         <v>150058521</v>
       </c>
       <c r="D12" t="s">
@@ -752,7 +820,7 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -760,7 +828,7 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -768,7 +836,7 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -776,7 +844,7 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -784,7 +852,7 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -792,15 +860,15 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -814,9 +882,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7">
+      <c r="A20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2">
         <v>86</v>
       </c>
       <c r="D20" t="s">
@@ -827,9 +895,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D21" t="s">
@@ -840,9 +908,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D22" t="s">
@@ -853,9 +921,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="7" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D23" t="s">
@@ -866,9 +934,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="7" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D24" t="s">
@@ -879,9 +947,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="7" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D25" t="s">
@@ -892,72 +960,206 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>33</v>
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="5"/>
+      <c r="C35">
+        <v>150</v>
+      </c>
+      <c r="D35" s="16">
+        <v>50000</v>
+      </c>
+      <c r="E35" s="16">
+        <v>7500000</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="5"/>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36" s="16">
+        <v>100000</v>
+      </c>
+      <c r="E36" s="16">
+        <v>5000000</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="5"/>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="16">
+        <v>50000</v>
+      </c>
+      <c r="E37" s="16">
+        <v>20000</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="5"/>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="16">
+        <v>20000</v>
+      </c>
+      <c r="E38" s="16">
+        <v>20000</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B39" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="40" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B34:B38"/>
     <mergeCell ref="B19:B25"/>
     <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A26:A30"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B8:B12"/>

</xml_diff>